<commit_message>
changes for second time
</commit_message>
<xml_diff>
--- a/src/test/resources/Test Data/Test Data.xlsx
+++ b/src/test/resources/Test Data/Test Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15270" windowHeight="6420" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15270" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="test_login" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,13 @@
     <sheet name="gotoOperational" sheetId="7" r:id="rId4"/>
     <sheet name="Vessel Master" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:E19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="54">
   <si>
     <t>WebElement</t>
   </si>
@@ -66,12 +67,6 @@
   </si>
   <si>
     <t>Logout</t>
-  </si>
-  <si>
-    <t>raypk</t>
-  </si>
-  <si>
-    <t>Homeserver@123</t>
   </si>
   <si>
     <t>//*[text()='User Name']/following-sibling::div/input</t>
@@ -559,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +569,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -597,18 +592,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -617,33 +609,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -661,9 +651,6 @@
       <formula1>"Id,Name,Xpath,LinkText,CSS,ClassName,PartialLinkText,TagName,NA"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -687,7 +674,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -710,16 +697,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -834,16 +821,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -851,16 +838,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -868,13 +855,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -885,16 +872,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -902,13 +889,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -941,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -956,7 +943,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -979,16 +966,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -999,16 +986,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -1019,10 +1006,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1039,16 +1026,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -1059,19 +1046,19 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1079,16 +1066,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -1099,7 +1086,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1119,19 +1106,19 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>